<commit_message>
made some changes into the code
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,54 +463,54 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>test.pdf</t>
+          <t>Feb 2022ST.pdf</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>16May2024</t>
+          <t>14/01/2022</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>221904111228</t>
+          <t>10904603</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>15:29:46</t>
+          <t>15:55:47</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>3.07</t>
+          <t>8.65</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>test.pdf</t>
+          <t>Feb 2022ST.pdf</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>01Jun2024</t>
+          <t>29/01/2022</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>221904111228</t>
+          <t>10904603</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>12:06:34</t>
+          <t>19:23:19</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2.67</t>
+          <t>8.56</t>
         </is>
       </c>
     </row>
@@ -522,7 +522,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>14/01/2022</t>
+          <t>10/02/2022</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -532,64 +532,10 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>15:55:47</t>
+          <t>15:08:04</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
-        <is>
-          <t>8.65</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Feb 2022ST.pdf</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>29/01/2022</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>10904603</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>19:23:19</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>8.56</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Feb 2022ST.pdf</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>10/02/2022</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>10904603</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>15:08:04</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
         <is>
           <t>8.56</t>
         </is>

</xml_diff>